<commit_message>
Optimalization of packet processing
</commit_message>
<xml_diff>
--- a/Performance Data.xlsx
+++ b/Performance Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Count</t>
   </si>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,14 +1091,34 @@
         <v>84839</v>
       </c>
     </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F18" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F19" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="F20" s="17">
+        <v>49</v>
+      </c>
+      <c r="G20" s="24">
+        <f>C5/F20</f>
+        <v>262.65306122448982</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1109,8 +1129,16 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="F21" s="17">
+        <v>1</v>
+      </c>
+      <c r="G21" s="24">
+        <f t="shared" ref="G21:G28" si="3">C6/F21</f>
+        <v>382</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1121,8 +1149,17 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="F22" s="17">
+        <v>41</v>
+      </c>
+      <c r="G22" s="24">
+        <f t="shared" si="3"/>
+        <v>546.09756097560978</v>
+      </c>
+      <c r="H22">
+        <f>AVERAGEA(G20:G28)</f>
+        <v>556.68124758452302</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1133,9 +1170,13 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="F23" s="17">
+        <v>2</v>
+      </c>
+      <c r="G23" s="24">
+        <f t="shared" si="3"/>
+        <v>680</v>
+      </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1146,9 +1187,16 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="F24" s="17">
+        <v>3</v>
+      </c>
+      <c r="G24" s="24">
+        <f t="shared" si="3"/>
+        <v>626.33333333333337</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -1159,9 +1207,17 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="F25" s="17">
+        <v>4</v>
+      </c>
+      <c r="G25" s="24">
+        <f t="shared" si="3"/>
+        <v>565.75</v>
+      </c>
+      <c r="H25">
+        <f>SUM(F20:F28)</f>
+        <v>167</v>
+      </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -1172,9 +1228,13 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="F26" s="17">
+        <v>22</v>
+      </c>
+      <c r="G26" s="24">
+        <f t="shared" si="3"/>
+        <v>648.22727272727275</v>
+      </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -1185,9 +1245,16 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="F27" s="17">
+        <v>20</v>
+      </c>
+      <c r="G27" s="24">
+        <f t="shared" si="3"/>
+        <v>608.54999999999995</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -1198,9 +1265,17 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="F28" s="17">
+        <v>25</v>
+      </c>
+      <c r="G28" s="24">
+        <f t="shared" si="3"/>
+        <v>690.52</v>
+      </c>
+      <c r="H28">
+        <f>D16/H25</f>
+        <v>508.01796407185628</v>
+      </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -1258,10 +1333,11 @@
       <c r="K32" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:L3"/>
+    <mergeCell ref="F18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Metadata storing in batches, configurable batch size
</commit_message>
<xml_diff>
--- a/Performance Data.xlsx
+++ b/Performance Data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Josefik\Master-Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Master-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SavePCAP_Cassandra" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t>Count</t>
   </si>
@@ -100,12 +100,27 @@
   </si>
   <si>
     <t>TODO: Add time for petsettisic.cap</t>
+  </si>
+  <si>
+    <t>host18_00046_20150613225816</t>
+  </si>
+  <si>
+    <t>host18_00047_20150615180251</t>
+  </si>
+  <si>
+    <t>host18_00049_20150619081334</t>
+  </si>
+  <si>
+    <t>host18_00053_20150701145004</t>
+  </si>
+  <si>
+    <t>host18_00054_20150703095345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -377,6 +392,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -690,11 +706,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +727,7 @@
     <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1320,11 +1336,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A7C734-72F4-4232-8F40-DD3E0A4CC0A0}">
-  <dimension ref="A3:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,9 +1353,12 @@
     <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>20</v>
       </c>
@@ -1351,8 +1370,13 @@
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="28"/>
+      <c r="N3" s="29"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1374,8 +1398,14 @@
       <c r="I4" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1386,7 +1416,7 @@
         <v>12870</v>
       </c>
       <c r="D5" s="16">
-        <f t="shared" ref="D5:D14" si="0">B5/C5</f>
+        <f t="shared" ref="D5:D13" si="0">B5/C5</f>
         <v>983.0438228438228</v>
       </c>
       <c r="F5" s="25">
@@ -1397,11 +1427,18 @@
         <v>32</v>
       </c>
       <c r="I5" s="17">
-        <f t="shared" ref="I5:I14" si="1">C5/H5</f>
+        <f t="shared" ref="I5:I13" si="1">C5/H5</f>
         <v>402.1875</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" s="13">
+        <v>20</v>
+      </c>
+      <c r="M5" s="17">
+        <f t="shared" ref="M5:M13" si="2">C5/L5</f>
+        <v>643.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -1425,8 +1462,18 @@
       <c r="J6" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="M6" s="17">
+        <f t="shared" si="2"/>
+        <v>382</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1454,8 +1501,19 @@
         <f>AVERAGEA(I5:I14)</f>
         <v>1690.9195987654321</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="13">
+        <v>10</v>
+      </c>
+      <c r="M7" s="17">
+        <f t="shared" si="2"/>
+        <v>2239</v>
+      </c>
+      <c r="N7">
+        <f>AVERAGEA(M5:M13)</f>
+        <v>2012.6722222222222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1480,8 +1538,15 @@
         <f t="shared" si="1"/>
         <v>1360</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="13">
+        <v>1</v>
+      </c>
+      <c r="M8" s="17">
+        <f t="shared" si="2"/>
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -1505,8 +1570,18 @@
       <c r="J9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" s="13">
+        <v>1</v>
+      </c>
+      <c r="M9" s="17">
+        <f t="shared" si="2"/>
+        <v>1879</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -1531,8 +1606,19 @@
         <f>SUM(H5:H14)</f>
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" s="13">
+        <v>1</v>
+      </c>
+      <c r="M10" s="17">
+        <f t="shared" si="2"/>
+        <v>2263</v>
+      </c>
+      <c r="N10">
+        <f>SUM(L5:L14)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -1553,8 +1639,15 @@
         <f t="shared" si="1"/>
         <v>2376.8333333333335</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" s="13">
+        <v>5</v>
+      </c>
+      <c r="M11" s="17">
+        <f t="shared" si="2"/>
+        <v>2852.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -1578,8 +1671,18 @@
       <c r="J12" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" s="13">
+        <v>4</v>
+      </c>
+      <c r="M12" s="17">
+        <f t="shared" si="2"/>
+        <v>3042.75</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>13</v>
       </c>
@@ -1604,8 +1707,19 @@
         <f>F8/J10</f>
         <v>1194.9154929577464</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13" s="13">
+        <v>5</v>
+      </c>
+      <c r="M13" s="17">
+        <f t="shared" si="2"/>
+        <v>3452.6</v>
+      </c>
+      <c r="N13">
+        <f>F8/N10</f>
+        <v>1767.4791666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="22"/>
       <c r="C14" s="19"/>
@@ -1613,11 +1727,53 @@
       <c r="H14" s="13"/>
       <c r="I14" s="23"/>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="30">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="30">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="30">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="30">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="30">
+        <v>500000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="H3:J3"/>
+    <mergeCell ref="L3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
How to, README, Performance Data
</commit_message>
<xml_diff>
--- a/Performance Data.xlsx
+++ b/Performance Data.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Master-Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Josefik\Master-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EB7A0E-02BB-4327-BF03-3BC8BF4C4ECA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SavePCAP_Cassandra" sheetId="1" r:id="rId1"/>
     <sheet name="SavePcap_Cassandra,MongoDB" sheetId="2" r:id="rId2"/>
+    <sheet name="SavePcap_BigData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="127">
   <si>
     <t>Count</t>
   </si>
@@ -102,25 +104,316 @@
     <t>TODO: Add time for petsettisic.cap</t>
   </si>
   <si>
-    <t>host18_00046_20150613225816</t>
-  </si>
-  <si>
-    <t>host18_00047_20150615180251</t>
-  </si>
-  <si>
-    <t>host18_00049_20150619081334</t>
-  </si>
-  <si>
-    <t>host18_00053_20150701145004</t>
-  </si>
-  <si>
-    <t>host18_00054_20150703095345</t>
+    <t>00000_20150420134956.cap</t>
+  </si>
+  <si>
+    <t>00001_20150421135456.cap</t>
+  </si>
+  <si>
+    <t>00002_20150421153149.cap</t>
+  </si>
+  <si>
+    <t>00003_20150421170839.cap</t>
+  </si>
+  <si>
+    <t>00004_20150421184241.cap</t>
+  </si>
+  <si>
+    <t>00005_20150421201655.cap</t>
+  </si>
+  <si>
+    <t>00006_20150421215224.cap</t>
+  </si>
+  <si>
+    <t>00007_20150422063358.cap</t>
+  </si>
+  <si>
+    <t>00008_20150422081005.cap</t>
+  </si>
+  <si>
+    <t>00009_20150422094425.cap</t>
+  </si>
+  <si>
+    <t>00010_20150422111834.cap</t>
+  </si>
+  <si>
+    <t>00011_20150422125713.cap</t>
+  </si>
+  <si>
+    <t>00012_20150422143344.cap</t>
+  </si>
+  <si>
+    <t>00013_20150422160848.cap</t>
+  </si>
+  <si>
+    <t>00014_20150422174444.cap</t>
+  </si>
+  <si>
+    <t>00015_20150422191809.cap</t>
+  </si>
+  <si>
+    <t>00016_20150422205528.cap</t>
+  </si>
+  <si>
+    <t>00017_20150422222842.cap</t>
+  </si>
+  <si>
+    <t>00018_20150423000156.cap</t>
+  </si>
+  <si>
+    <t>00019_20150423013710.cap</t>
+  </si>
+  <si>
+    <t>00020_20150423031027.cap</t>
+  </si>
+  <si>
+    <t>00021_20150423044408.cap</t>
+  </si>
+  <si>
+    <t>00022_20150423061741.cap</t>
+  </si>
+  <si>
+    <t>00023_20150423075101.cap</t>
+  </si>
+  <si>
+    <t>00024_20150423092626.cap</t>
+  </si>
+  <si>
+    <t>00025_20150423110449.cap</t>
+  </si>
+  <si>
+    <t>00026_20150426033314.cap</t>
+  </si>
+  <si>
+    <t>00027_20150428154946.cap</t>
+  </si>
+  <si>
+    <t>00028_20150507215957.cap</t>
+  </si>
+  <si>
+    <t>00029_20150509035842.cap</t>
+  </si>
+  <si>
+    <t>00030_20150512120718.cap</t>
+  </si>
+  <si>
+    <t>00031_20150514132945.cap</t>
+  </si>
+  <si>
+    <t>00032_20150517100954.cap</t>
+  </si>
+  <si>
+    <t>00033_20150519010341.cap</t>
+  </si>
+  <si>
+    <t>00034_20150521013723.cap</t>
+  </si>
+  <si>
+    <t>00035_20150523151214.cap</t>
+  </si>
+  <si>
+    <t>00036_20150525101628.cap</t>
+  </si>
+  <si>
+    <t>00037_20150527052220.cap</t>
+  </si>
+  <si>
+    <t>00038_20150529002616.cap</t>
+  </si>
+  <si>
+    <t>00039_20150530193046.cap</t>
+  </si>
+  <si>
+    <t>00040_20150601144038.cap</t>
+  </si>
+  <si>
+    <t>00041_20150603094527.cap</t>
+  </si>
+  <si>
+    <t>00042_20150605045007.cap</t>
+  </si>
+  <si>
+    <t>00043_20150606235449.cap</t>
+  </si>
+  <si>
+    <t>00044_20150608190519.cap</t>
+  </si>
+  <si>
+    <t>00045_20150611031812.cap</t>
+  </si>
+  <si>
+    <t>00046_20150613225816.cap</t>
+  </si>
+  <si>
+    <t>00047_20150615180251.cap</t>
+  </si>
+  <si>
+    <t>00048_20150617130703.cap</t>
+  </si>
+  <si>
+    <t>00049_20150619081334.cap</t>
+  </si>
+  <si>
+    <t>00050_20150621031754.cap</t>
+  </si>
+  <si>
+    <t>00051_20150625080919.cap</t>
+  </si>
+  <si>
+    <t>00052_20150629193952.cap</t>
+  </si>
+  <si>
+    <t>00053_20150701145004.cap</t>
+  </si>
+  <si>
+    <t>00054_20150703095345.cap</t>
+  </si>
+  <si>
+    <t>00055_20150705045741.cap</t>
+  </si>
+  <si>
+    <t>00056_20150707000238.cap</t>
+  </si>
+  <si>
+    <t>00057_20150710051119.cap</t>
+  </si>
+  <si>
+    <t>00058_20150714025042.cap</t>
+  </si>
+  <si>
+    <t>00059_20150717063929.cap</t>
+  </si>
+  <si>
+    <t>00060_20150721015935.cap</t>
+  </si>
+  <si>
+    <t>00061_20150723021627.cap</t>
+  </si>
+  <si>
+    <t>00062_20150725112419.cap</t>
+  </si>
+  <si>
+    <t>00063_20150728175149.cap</t>
+  </si>
+  <si>
+    <t>00064_20150730202110.cap</t>
+  </si>
+  <si>
+    <t>00065_20150802060904.cap</t>
+  </si>
+  <si>
+    <t>00066_20150804140310.cap</t>
+  </si>
+  <si>
+    <t>00067_20150805165341.cap</t>
+  </si>
+  <si>
+    <t>00068_20150807125157.cap</t>
+  </si>
+  <si>
+    <t>00069_20150809112821.cap</t>
+  </si>
+  <si>
+    <t>00070_20150811000849.cap</t>
+  </si>
+  <si>
+    <t>00071_20150812034936.cap</t>
+  </si>
+  <si>
+    <t>00072_20150814111246.cap</t>
+  </si>
+  <si>
+    <t>00073_20150815211946.cap</t>
+  </si>
+  <si>
+    <t>00074_20150817164817.cap</t>
+  </si>
+  <si>
+    <t>00075_20150819094423.cap</t>
+  </si>
+  <si>
+    <t>00076_20150820155511.cap</t>
+  </si>
+  <si>
+    <t>00077_20150821150607.cap</t>
+  </si>
+  <si>
+    <t>00078_20150822103348.cap</t>
+  </si>
+  <si>
+    <t>00079_20150823205729.cap</t>
+  </si>
+  <si>
+    <t>00080_20150825093737.cap</t>
+  </si>
+  <si>
+    <t>00081_20150826071714.cap</t>
+  </si>
+  <si>
+    <t>00082_20150828024744.cap</t>
+  </si>
+  <si>
+    <t>00083_20150829144424.cap</t>
+  </si>
+  <si>
+    <t>00084_20150901195110.cap</t>
+  </si>
+  <si>
+    <t>00085_20150903163645.cap</t>
+  </si>
+  <si>
+    <t>00086_20150907160533.cap</t>
+  </si>
+  <si>
+    <t>00087_20150911231543.cap</t>
+  </si>
+  <si>
+    <t>00088_20150916140709.cap</t>
+  </si>
+  <si>
+    <t>00089_20150919102102.cap</t>
+  </si>
+  <si>
+    <t>00090_20150924014129.cap</t>
+  </si>
+  <si>
+    <t>00091_20150926111839.cap</t>
+  </si>
+  <si>
+    <t>00092_20150929153928.cap</t>
+  </si>
+  <si>
+    <t>00093_20151005000758.cap</t>
+  </si>
+  <si>
+    <t>00094_20151009184528.cap</t>
+  </si>
+  <si>
+    <t>00095_20151015011034.cap</t>
+  </si>
+  <si>
+    <t>00096_20151021223922.cap</t>
+  </si>
+  <si>
+    <t>00097_20151103133033.cap</t>
+  </si>
+  <si>
+    <t>00098_20151122161242.cap</t>
+  </si>
+  <si>
+    <t>00099_20151211185234.cap</t>
+  </si>
+  <si>
+    <t>00100_20151230213514.cap</t>
+  </si>
+  <si>
+    <t>00101_20160119001814.cap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,7 +471,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -313,11 +606,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -392,6 +718,29 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,7 +1055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1336,11 +1685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,45 +2076,20 @@
       <c r="H14" s="13"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="27">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="27">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="27">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="27">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="27">
-        <v>500000</v>
-      </c>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="27"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="27"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="27"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1776,4 +2100,1581 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A40B2E-1797-406B-8C91-F3814EB24900}">
+  <dimension ref="A3:D106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="37">
+        <v>97661950</v>
+      </c>
+      <c r="C5" s="37">
+        <v>500000</v>
+      </c>
+      <c r="D5" s="35">
+        <f>B5/C5</f>
+        <v>195.32390000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="38">
+        <v>95806099</v>
+      </c>
+      <c r="C6" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D6" s="22">
+        <f t="shared" ref="D6:D69" si="0">B6/C6</f>
+        <v>191.61219800000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="38">
+        <v>95858806</v>
+      </c>
+      <c r="C7" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D7" s="22">
+        <f t="shared" si="0"/>
+        <v>191.717612</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="38">
+        <v>95804731</v>
+      </c>
+      <c r="C8" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D8" s="22">
+        <f t="shared" si="0"/>
+        <v>191.60946200000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="38">
+        <v>95831946</v>
+      </c>
+      <c r="C9" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D9" s="22">
+        <f t="shared" si="0"/>
+        <v>191.663892</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="38">
+        <v>95717636</v>
+      </c>
+      <c r="C10" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D10" s="22">
+        <f t="shared" si="0"/>
+        <v>191.435272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="38">
+        <v>95835021</v>
+      </c>
+      <c r="C11" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D11" s="22">
+        <f t="shared" si="0"/>
+        <v>191.670042</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="38">
+        <v>95751991</v>
+      </c>
+      <c r="C12" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D12" s="22">
+        <f t="shared" si="0"/>
+        <v>191.50398200000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="38">
+        <v>95783362</v>
+      </c>
+      <c r="C13" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D13" s="22">
+        <f t="shared" si="0"/>
+        <v>191.56672399999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="38">
+        <v>95883508</v>
+      </c>
+      <c r="C14" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D14" s="22">
+        <f t="shared" si="0"/>
+        <v>191.76701600000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="38">
+        <v>95823448</v>
+      </c>
+      <c r="C15" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D15" s="22">
+        <f t="shared" si="0"/>
+        <v>191.646896</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="38">
+        <v>95818589</v>
+      </c>
+      <c r="C16" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D16" s="22">
+        <f t="shared" si="0"/>
+        <v>191.63717800000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="38">
+        <v>95759175</v>
+      </c>
+      <c r="C17" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D17" s="22">
+        <f t="shared" si="0"/>
+        <v>191.51835</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="38">
+        <v>95876439</v>
+      </c>
+      <c r="C18" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D18" s="22">
+        <f t="shared" si="0"/>
+        <v>191.75287800000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="38">
+        <v>95829535</v>
+      </c>
+      <c r="C19" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D19" s="22">
+        <f t="shared" si="0"/>
+        <v>191.65907000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="38">
+        <v>95796943</v>
+      </c>
+      <c r="C20" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D20" s="22">
+        <f t="shared" si="0"/>
+        <v>191.593886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="38">
+        <v>95685466</v>
+      </c>
+      <c r="C21" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D21" s="22">
+        <f t="shared" si="0"/>
+        <v>191.37093200000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="38">
+        <v>95708916</v>
+      </c>
+      <c r="C22" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D22" s="22">
+        <f t="shared" si="0"/>
+        <v>191.417832</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="38">
+        <v>95803070</v>
+      </c>
+      <c r="C23" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D23" s="22">
+        <f t="shared" si="0"/>
+        <v>191.60614000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="38">
+        <v>95802651</v>
+      </c>
+      <c r="C24" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D24" s="22">
+        <f t="shared" si="0"/>
+        <v>191.60530199999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="38">
+        <v>95622380</v>
+      </c>
+      <c r="C25" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D25" s="22">
+        <f t="shared" si="0"/>
+        <v>191.24476000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="38">
+        <v>95753452</v>
+      </c>
+      <c r="C26" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D26" s="22">
+        <f t="shared" si="0"/>
+        <v>191.50690399999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="38">
+        <v>95932534</v>
+      </c>
+      <c r="C27" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D27" s="22">
+        <f t="shared" si="0"/>
+        <v>191.86506800000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="38">
+        <v>95941193</v>
+      </c>
+      <c r="C28" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D28" s="22">
+        <f t="shared" si="0"/>
+        <v>191.882386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="38">
+        <v>95366566</v>
+      </c>
+      <c r="C29" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D29" s="22">
+        <f t="shared" si="0"/>
+        <v>190.73313200000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="38">
+        <v>109666255</v>
+      </c>
+      <c r="C30" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D30" s="22">
+        <f t="shared" si="0"/>
+        <v>219.33251000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="38">
+        <v>111164928</v>
+      </c>
+      <c r="C31" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D31" s="22">
+        <f t="shared" si="0"/>
+        <v>222.32985600000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="38">
+        <v>126030611</v>
+      </c>
+      <c r="C32" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D32" s="22">
+        <f t="shared" si="0"/>
+        <v>252.06122199999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="38">
+        <v>90956436</v>
+      </c>
+      <c r="C33" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D33" s="22">
+        <f t="shared" si="0"/>
+        <v>181.91287199999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="38">
+        <v>122418798</v>
+      </c>
+      <c r="C34" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D34" s="22">
+        <f t="shared" si="0"/>
+        <v>244.83759599999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="38">
+        <v>245722681</v>
+      </c>
+      <c r="C35" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D35" s="22">
+        <f t="shared" si="0"/>
+        <v>491.44536199999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="38">
+        <v>107832997</v>
+      </c>
+      <c r="C36" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D36" s="22">
+        <f t="shared" si="0"/>
+        <v>215.66599400000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="38">
+        <v>82511212</v>
+      </c>
+      <c r="C37" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D37" s="22">
+        <f t="shared" si="0"/>
+        <v>165.022424</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="38">
+        <v>99396146</v>
+      </c>
+      <c r="C38" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D38" s="22">
+        <f t="shared" si="0"/>
+        <v>198.792292</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="38">
+        <v>86448326</v>
+      </c>
+      <c r="C39" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D39" s="22">
+        <f t="shared" si="0"/>
+        <v>172.89665199999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="38">
+        <v>69929499</v>
+      </c>
+      <c r="C40" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D40" s="22">
+        <f t="shared" si="0"/>
+        <v>139.85899800000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="38">
+        <v>69939538</v>
+      </c>
+      <c r="C41" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D41" s="22">
+        <f t="shared" si="0"/>
+        <v>139.879076</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="38">
+        <v>69934497</v>
+      </c>
+      <c r="C42" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D42" s="22">
+        <f t="shared" si="0"/>
+        <v>139.86899399999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="38">
+        <v>69936203</v>
+      </c>
+      <c r="C43" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D43" s="22">
+        <f t="shared" si="0"/>
+        <v>139.87240600000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="38">
+        <v>69970313</v>
+      </c>
+      <c r="C44" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D44" s="22">
+        <f t="shared" si="0"/>
+        <v>139.94062600000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="38">
+        <v>69940096</v>
+      </c>
+      <c r="C45" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D45" s="22">
+        <f t="shared" si="0"/>
+        <v>139.88019199999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="38">
+        <v>69931107</v>
+      </c>
+      <c r="C46" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D46" s="22">
+        <f t="shared" si="0"/>
+        <v>139.86221399999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="38">
+        <v>69937712</v>
+      </c>
+      <c r="C47" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D47" s="22">
+        <f t="shared" si="0"/>
+        <v>139.87542400000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="38">
+        <v>69972723</v>
+      </c>
+      <c r="C48" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D48" s="22">
+        <f t="shared" si="0"/>
+        <v>139.945446</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="38">
+        <v>77575286</v>
+      </c>
+      <c r="C49" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D49" s="22">
+        <f t="shared" si="0"/>
+        <v>155.15057200000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="38">
+        <v>84198846</v>
+      </c>
+      <c r="C50" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D50" s="22">
+        <f t="shared" si="0"/>
+        <v>168.39769200000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="38">
+        <v>69905384</v>
+      </c>
+      <c r="C51" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D51" s="22">
+        <f t="shared" si="0"/>
+        <v>139.810768</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" s="38">
+        <v>69909786</v>
+      </c>
+      <c r="C52" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D52" s="22">
+        <f t="shared" si="0"/>
+        <v>139.81957199999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="38">
+        <v>69919169</v>
+      </c>
+      <c r="C53" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D53" s="22">
+        <f t="shared" si="0"/>
+        <v>139.83833799999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="38">
+        <v>69901238</v>
+      </c>
+      <c r="C54" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D54" s="22">
+        <f t="shared" si="0"/>
+        <v>139.80247600000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="38">
+        <v>93464633</v>
+      </c>
+      <c r="C55" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D55" s="22">
+        <f t="shared" si="0"/>
+        <v>186.92926600000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="38">
+        <v>104525166</v>
+      </c>
+      <c r="C56" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D56" s="22">
+        <f t="shared" si="0"/>
+        <v>209.050332</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="38">
+        <v>69951861</v>
+      </c>
+      <c r="C57" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D57" s="22">
+        <f t="shared" si="0"/>
+        <v>139.90372199999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B58" s="38">
+        <v>69915198</v>
+      </c>
+      <c r="C58" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D58" s="22">
+        <f t="shared" si="0"/>
+        <v>139.83039600000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="38">
+        <v>69916773</v>
+      </c>
+      <c r="C59" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D59" s="22">
+        <f t="shared" si="0"/>
+        <v>139.83354600000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" s="38">
+        <v>69922018</v>
+      </c>
+      <c r="C60" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D60" s="22">
+        <f t="shared" si="0"/>
+        <v>139.84403599999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="38">
+        <v>94901338</v>
+      </c>
+      <c r="C61" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D61" s="22">
+        <f t="shared" si="0"/>
+        <v>189.80267599999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" s="38">
+        <v>114297440</v>
+      </c>
+      <c r="C62" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D62" s="22">
+        <f t="shared" si="0"/>
+        <v>228.59487999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" s="38">
+        <v>107262171</v>
+      </c>
+      <c r="C63" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D63" s="22">
+        <f t="shared" si="0"/>
+        <v>214.52434199999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="38">
+        <v>114737314</v>
+      </c>
+      <c r="C64" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D64" s="22">
+        <f t="shared" si="0"/>
+        <v>229.474628</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="38">
+        <v>99686925</v>
+      </c>
+      <c r="C65" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D65" s="22">
+        <f t="shared" si="0"/>
+        <v>199.37385</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="38">
+        <v>105947634</v>
+      </c>
+      <c r="C66" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D66" s="22">
+        <f t="shared" si="0"/>
+        <v>211.89526799999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="38">
+        <v>112424850</v>
+      </c>
+      <c r="C67" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D67" s="22">
+        <f t="shared" si="0"/>
+        <v>224.84970000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="38">
+        <v>103454867</v>
+      </c>
+      <c r="C68" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D68" s="22">
+        <f t="shared" si="0"/>
+        <v>206.90973399999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" s="38">
+        <v>105195383</v>
+      </c>
+      <c r="C69" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D69" s="22">
+        <f t="shared" si="0"/>
+        <v>210.39076600000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B70" s="38">
+        <v>103821763</v>
+      </c>
+      <c r="C70" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D70" s="22">
+        <f t="shared" ref="D70:D106" si="1">B70/C70</f>
+        <v>207.64352600000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" s="38">
+        <v>91035050</v>
+      </c>
+      <c r="C71" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D71" s="22">
+        <f t="shared" si="1"/>
+        <v>182.0701</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="38">
+        <v>99498163</v>
+      </c>
+      <c r="C72" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D72" s="22">
+        <f t="shared" si="1"/>
+        <v>198.99632600000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="38">
+        <v>102292773</v>
+      </c>
+      <c r="C73" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D73" s="22">
+        <f t="shared" si="1"/>
+        <v>204.58554599999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="38">
+        <v>98777448</v>
+      </c>
+      <c r="C74" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D74" s="22">
+        <f t="shared" si="1"/>
+        <v>197.55489600000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="38">
+        <v>92426745</v>
+      </c>
+      <c r="C75" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D75" s="22">
+        <f t="shared" si="1"/>
+        <v>184.85348999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="38">
+        <v>105949676</v>
+      </c>
+      <c r="C76" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D76" s="22">
+        <f t="shared" si="1"/>
+        <v>211.89935199999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" s="38">
+        <v>99195546</v>
+      </c>
+      <c r="C77" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D77" s="22">
+        <f t="shared" si="1"/>
+        <v>198.39109199999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B78" s="38">
+        <v>100381998</v>
+      </c>
+      <c r="C78" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D78" s="22">
+        <f t="shared" si="1"/>
+        <v>200.76399599999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" s="38">
+        <v>101379736</v>
+      </c>
+      <c r="C79" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D79" s="22">
+        <f t="shared" si="1"/>
+        <v>202.75947199999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" s="38">
+        <v>97241294</v>
+      </c>
+      <c r="C80" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D80" s="22">
+        <f t="shared" si="1"/>
+        <v>194.48258799999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" s="38">
+        <v>90319402</v>
+      </c>
+      <c r="C81" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D81" s="22">
+        <f t="shared" si="1"/>
+        <v>180.63880399999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82" s="38">
+        <v>90642493</v>
+      </c>
+      <c r="C82" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D82" s="22">
+        <f t="shared" si="1"/>
+        <v>181.284986</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="38">
+        <v>97537714</v>
+      </c>
+      <c r="C83" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D83" s="22">
+        <f t="shared" si="1"/>
+        <v>195.07542799999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" s="38">
+        <v>98884601</v>
+      </c>
+      <c r="C84" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D84" s="22">
+        <f t="shared" si="1"/>
+        <v>197.76920200000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="38">
+        <v>91902456</v>
+      </c>
+      <c r="C85" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D85" s="22">
+        <f t="shared" si="1"/>
+        <v>183.804912</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B86" s="38">
+        <v>99851880</v>
+      </c>
+      <c r="C86" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D86" s="22">
+        <f t="shared" si="1"/>
+        <v>199.70375999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" s="38">
+        <v>97182369</v>
+      </c>
+      <c r="C87" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D87" s="22">
+        <f t="shared" si="1"/>
+        <v>194.36473799999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B88" s="38">
+        <v>111682088</v>
+      </c>
+      <c r="C88" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D88" s="22">
+        <f t="shared" si="1"/>
+        <v>223.36417599999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B89" s="38">
+        <v>97228019</v>
+      </c>
+      <c r="C89" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D89" s="22">
+        <f t="shared" si="1"/>
+        <v>194.45603800000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" s="38">
+        <v>116928690</v>
+      </c>
+      <c r="C90" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D90" s="22">
+        <f t="shared" si="1"/>
+        <v>233.85738000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91" s="38">
+        <v>238350844</v>
+      </c>
+      <c r="C91" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D91" s="22">
+        <f t="shared" si="1"/>
+        <v>476.70168799999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B92" s="38">
+        <v>119463297</v>
+      </c>
+      <c r="C92" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D92" s="22">
+        <f t="shared" si="1"/>
+        <v>238.92659399999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B93" s="38">
+        <v>189803147</v>
+      </c>
+      <c r="C93" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D93" s="22">
+        <f t="shared" si="1"/>
+        <v>379.60629399999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94" s="38">
+        <v>233229533</v>
+      </c>
+      <c r="C94" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D94" s="22">
+        <f t="shared" si="1"/>
+        <v>466.45906600000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B95" s="38">
+        <v>218441522</v>
+      </c>
+      <c r="C95" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D95" s="22">
+        <f t="shared" si="1"/>
+        <v>436.88304399999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B96" s="38">
+        <v>216072658</v>
+      </c>
+      <c r="C96" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D96" s="22">
+        <f t="shared" si="1"/>
+        <v>432.14531599999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B97" s="38">
+        <v>134970172</v>
+      </c>
+      <c r="C97" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D97" s="22">
+        <f t="shared" si="1"/>
+        <v>269.94034399999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" s="38">
+        <v>107431604</v>
+      </c>
+      <c r="C98" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D98" s="22">
+        <f t="shared" si="1"/>
+        <v>214.86320799999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B99" s="38">
+        <v>113652706</v>
+      </c>
+      <c r="C99" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D99" s="22">
+        <f t="shared" si="1"/>
+        <v>227.30541199999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B100" s="38">
+        <v>158672195</v>
+      </c>
+      <c r="C100" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D100" s="22">
+        <f t="shared" si="1"/>
+        <v>317.34438999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B101" s="38">
+        <v>283750086</v>
+      </c>
+      <c r="C101" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D101" s="22">
+        <f t="shared" si="1"/>
+        <v>567.50017200000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B102" s="38">
+        <v>206954008</v>
+      </c>
+      <c r="C102" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D102" s="22">
+        <f t="shared" si="1"/>
+        <v>413.90801599999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B103" s="38">
+        <v>206952024</v>
+      </c>
+      <c r="C103" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D103" s="22">
+        <f t="shared" si="1"/>
+        <v>413.90404799999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B104" s="38">
+        <v>206960360</v>
+      </c>
+      <c r="C104" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D104" s="22">
+        <f t="shared" si="1"/>
+        <v>413.92072000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B105" s="38">
+        <v>206968130</v>
+      </c>
+      <c r="C105" s="38">
+        <v>500000</v>
+      </c>
+      <c r="D105" s="22">
+        <f t="shared" si="1"/>
+        <v>413.93626</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B106" s="39">
+        <v>145543574</v>
+      </c>
+      <c r="C106" s="39">
+        <v>500000</v>
+      </c>
+      <c r="D106" s="36">
+        <f t="shared" si="1"/>
+        <v>291.08714800000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update - see description
- Refactored package for Handlers
- Removed TestDatabaseSpringBoot
- PerformanceData.xlsx
</commit_message>
<xml_diff>
--- a/Performance Data.xlsx
+++ b/Performance Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Josefik\Master-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EB7A0E-02BB-4327-BF03-3BC8BF4C4ECA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BBC335-751F-4F37-A452-1F911536AEF3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="127">
   <si>
     <t>Count</t>
   </si>
@@ -643,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -710,15 +710,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -741,6 +732,21 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1085,22 +1091,22 @@
       <c r="F1" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="H3" s="28" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="H3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30"/>
-      <c r="L3" s="28" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
+      <c r="L3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="39"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
@@ -1689,7 +1695,7 @@
   <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,22 +1714,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="H3" s="28" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="H3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30"/>
-      <c r="L3" s="28" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
+      <c r="L3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="39"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1847,7 +1853,7 @@
         <v>1243.8888888888889</v>
       </c>
       <c r="J7">
-        <f>AVERAGEA(I5:I14)</f>
+        <f>AVERAGEA(I5:I13)</f>
         <v>1690.9195987654321</v>
       </c>
       <c r="L7" s="13">
@@ -2104,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A40B2E-1797-406B-8C91-F3814EB24900}">
-  <dimension ref="A3:D106"/>
+  <dimension ref="A3:L106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,17 +2122,23 @@
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2139,1540 +2151,2288 @@
       <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="E4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="34">
         <v>97661950</v>
       </c>
-      <c r="C5" s="37">
-        <v>500000</v>
-      </c>
-      <c r="D5" s="35">
+      <c r="C5" s="34">
+        <v>500000</v>
+      </c>
+      <c r="D5" s="32">
         <f>B5/C5</f>
         <v>195.32390000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="30">
+        <v>28</v>
+      </c>
+      <c r="F5" s="30">
+        <f>C5/E5</f>
+        <v>17857.142857142859</v>
+      </c>
+      <c r="L5" s="25">
+        <f>AVERAGEA(D5:D106)</f>
+        <v>218.75459860784309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="35">
         <v>95806099</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="35">
         <v>500000</v>
       </c>
       <c r="D6" s="22">
         <f t="shared" ref="D6:D69" si="0">B6/C6</f>
         <v>191.61219800000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="30">
+        <v>28</v>
+      </c>
+      <c r="F6" s="30">
+        <f t="shared" ref="F6:F69" si="1">C6/E6</f>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7" s="35">
         <v>95858806</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="35">
         <v>500000</v>
       </c>
       <c r="D7" s="22">
         <f t="shared" si="0"/>
         <v>191.717612</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="30">
+        <v>28</v>
+      </c>
+      <c r="F7" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="35">
         <v>95804731</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="35">
         <v>500000</v>
       </c>
       <c r="D8" s="22">
         <f t="shared" si="0"/>
         <v>191.60946200000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="30">
+        <v>28</v>
+      </c>
+      <c r="F8" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+      <c r="L8" s="24">
+        <f>SUM(C5:C106)</f>
+        <v>51000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="38">
+      <c r="B9" s="35">
         <v>95831946</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="35">
         <v>500000</v>
       </c>
       <c r="D9" s="22">
         <f t="shared" si="0"/>
         <v>191.663892</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="30">
+        <v>28</v>
+      </c>
+      <c r="F9" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="35">
         <v>95717636</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="35">
         <v>500000</v>
       </c>
       <c r="D10" s="22">
         <f t="shared" si="0"/>
         <v>191.435272</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="30">
+        <v>28</v>
+      </c>
+      <c r="F10" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="35">
         <v>95835021</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="35">
         <v>500000</v>
       </c>
       <c r="D11" s="22">
         <f t="shared" si="0"/>
         <v>191.670042</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="30">
+        <v>28</v>
+      </c>
+      <c r="F11" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+      <c r="L11" s="31">
+        <f>AVERAGEA(F5:F106)</f>
+        <v>17857.142857142891</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="38">
+      <c r="B12" s="35">
         <v>95751991</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="35">
         <v>500000</v>
       </c>
       <c r="D12" s="22">
         <f t="shared" si="0"/>
         <v>191.50398200000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="30">
+        <v>28</v>
+      </c>
+      <c r="F12" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="38">
+      <c r="B13" s="35">
         <v>95783362</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="35">
         <v>500000</v>
       </c>
       <c r="D13" s="22">
         <f t="shared" si="0"/>
         <v>191.56672399999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="E13" s="30">
+        <v>28</v>
+      </c>
+      <c r="F13" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="38">
+      <c r="B14" s="35">
         <v>95883508</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="35">
         <v>500000</v>
       </c>
       <c r="D14" s="22">
         <f t="shared" si="0"/>
         <v>191.76701600000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="E14" s="30">
+        <v>28</v>
+      </c>
+      <c r="F14" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+      <c r="L14" s="31">
+        <f>SUM(E5:E106)</f>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="38">
+      <c r="B15" s="35">
         <v>95823448</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="35">
         <v>500000</v>
       </c>
       <c r="D15" s="22">
         <f t="shared" si="0"/>
         <v>191.646896</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="E15" s="30">
+        <v>28</v>
+      </c>
+      <c r="F15" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="35">
         <v>95818589</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="35">
         <v>500000</v>
       </c>
       <c r="D16" s="22">
         <f t="shared" si="0"/>
         <v>191.63717800000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="E16" s="30">
+        <v>28</v>
+      </c>
+      <c r="F16" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17" s="35">
         <v>95759175</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="35">
         <v>500000</v>
       </c>
       <c r="D17" s="22">
         <f t="shared" si="0"/>
         <v>191.51835</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="E17" s="30">
+        <v>28</v>
+      </c>
+      <c r="F17" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="38">
+      <c r="B18" s="35">
         <v>95876439</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="35">
         <v>500000</v>
       </c>
       <c r="D18" s="22">
         <f t="shared" si="0"/>
         <v>191.75287800000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="E18" s="30">
+        <v>28</v>
+      </c>
+      <c r="F18" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="35">
         <v>95829535</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="35">
         <v>500000</v>
       </c>
       <c r="D19" s="22">
         <f t="shared" si="0"/>
         <v>191.65907000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="E19" s="30">
+        <v>28</v>
+      </c>
+      <c r="F19" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="38">
+      <c r="B20" s="35">
         <v>95796943</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="35">
         <v>500000</v>
       </c>
       <c r="D20" s="22">
         <f t="shared" si="0"/>
         <v>191.593886</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="E20" s="30">
+        <v>28</v>
+      </c>
+      <c r="F20" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="38">
+      <c r="B21" s="35">
         <v>95685466</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="35">
         <v>500000</v>
       </c>
       <c r="D21" s="22">
         <f t="shared" si="0"/>
         <v>191.37093200000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="E21" s="30">
+        <v>28</v>
+      </c>
+      <c r="F21" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="38">
+      <c r="B22" s="35">
         <v>95708916</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="35">
         <v>500000</v>
       </c>
       <c r="D22" s="22">
         <f t="shared" si="0"/>
         <v>191.417832</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="E22" s="30">
+        <v>28</v>
+      </c>
+      <c r="F22" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="35">
         <v>95803070</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="35">
         <v>500000</v>
       </c>
       <c r="D23" s="22">
         <f t="shared" si="0"/>
         <v>191.60614000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="E23" s="30">
+        <v>28</v>
+      </c>
+      <c r="F23" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="38">
+      <c r="B24" s="35">
         <v>95802651</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="35">
         <v>500000</v>
       </c>
       <c r="D24" s="22">
         <f t="shared" si="0"/>
         <v>191.60530199999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="E24" s="30">
+        <v>28</v>
+      </c>
+      <c r="F24" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B25" s="35">
         <v>95622380</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="35">
         <v>500000</v>
       </c>
       <c r="D25" s="22">
         <f t="shared" si="0"/>
         <v>191.24476000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="E25" s="30">
+        <v>28</v>
+      </c>
+      <c r="F25" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="38">
+      <c r="B26" s="35">
         <v>95753452</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C26" s="35">
         <v>500000</v>
       </c>
       <c r="D26" s="22">
         <f t="shared" si="0"/>
         <v>191.50690399999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="E26" s="30">
+        <v>28</v>
+      </c>
+      <c r="F26" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="38">
+      <c r="B27" s="35">
         <v>95932534</v>
       </c>
-      <c r="C27" s="38">
+      <c r="C27" s="35">
         <v>500000</v>
       </c>
       <c r="D27" s="22">
         <f t="shared" si="0"/>
         <v>191.86506800000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="E27" s="30">
+        <v>28</v>
+      </c>
+      <c r="F27" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="38">
+      <c r="B28" s="35">
         <v>95941193</v>
       </c>
-      <c r="C28" s="38">
+      <c r="C28" s="35">
         <v>500000</v>
       </c>
       <c r="D28" s="22">
         <f t="shared" si="0"/>
         <v>191.882386</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+      <c r="E28" s="30">
+        <v>28</v>
+      </c>
+      <c r="F28" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29" s="35">
         <v>95366566</v>
       </c>
-      <c r="C29" s="38">
+      <c r="C29" s="35">
         <v>500000</v>
       </c>
       <c r="D29" s="22">
         <f t="shared" si="0"/>
         <v>190.73313200000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+      <c r="E29" s="30">
+        <v>28</v>
+      </c>
+      <c r="F29" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="35">
         <v>109666255</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="35">
         <v>500000</v>
       </c>
       <c r="D30" s="22">
         <f t="shared" si="0"/>
         <v>219.33251000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="E30" s="30">
+        <v>28</v>
+      </c>
+      <c r="F30" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="38">
+      <c r="B31" s="35">
         <v>111164928</v>
       </c>
-      <c r="C31" s="38">
+      <c r="C31" s="35">
         <v>500000</v>
       </c>
       <c r="D31" s="22">
         <f t="shared" si="0"/>
         <v>222.32985600000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="E31" s="30">
+        <v>28</v>
+      </c>
+      <c r="F31" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="38">
+      <c r="B32" s="35">
         <v>126030611</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C32" s="35">
         <v>500000</v>
       </c>
       <c r="D32" s="22">
         <f t="shared" si="0"/>
         <v>252.06122199999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="E32" s="30">
+        <v>28</v>
+      </c>
+      <c r="F32" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="35">
         <v>90956436</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="35">
         <v>500000</v>
       </c>
       <c r="D33" s="22">
         <f t="shared" si="0"/>
         <v>181.91287199999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="E33" s="30">
+        <v>28</v>
+      </c>
+      <c r="F33" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="38">
+      <c r="B34" s="35">
         <v>122418798</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="35">
         <v>500000</v>
       </c>
       <c r="D34" s="22">
         <f t="shared" si="0"/>
         <v>244.83759599999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+      <c r="E34" s="30">
+        <v>28</v>
+      </c>
+      <c r="F34" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="38">
+      <c r="B35" s="35">
         <v>245722681</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C35" s="35">
         <v>500000</v>
       </c>
       <c r="D35" s="22">
         <f t="shared" si="0"/>
         <v>491.44536199999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="E35" s="30">
+        <v>28</v>
+      </c>
+      <c r="F35" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="38">
+      <c r="B36" s="35">
         <v>107832997</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="35">
         <v>500000</v>
       </c>
       <c r="D36" s="22">
         <f t="shared" si="0"/>
         <v>215.66599400000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="E36" s="30">
+        <v>28</v>
+      </c>
+      <c r="F36" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="38">
+      <c r="B37" s="35">
         <v>82511212</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="35">
         <v>500000</v>
       </c>
       <c r="D37" s="22">
         <f t="shared" si="0"/>
         <v>165.022424</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+      <c r="E37" s="30">
+        <v>28</v>
+      </c>
+      <c r="F37" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="38">
+      <c r="B38" s="35">
         <v>99396146</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="35">
         <v>500000</v>
       </c>
       <c r="D38" s="22">
         <f t="shared" si="0"/>
         <v>198.792292</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="E38" s="30">
+        <v>28</v>
+      </c>
+      <c r="F38" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="38">
+      <c r="B39" s="35">
         <v>86448326</v>
       </c>
-      <c r="C39" s="38">
+      <c r="C39" s="35">
         <v>500000</v>
       </c>
       <c r="D39" s="22">
         <f t="shared" si="0"/>
         <v>172.89665199999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
+      <c r="E39" s="30">
+        <v>28</v>
+      </c>
+      <c r="F39" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="38">
+      <c r="B40" s="35">
         <v>69929499</v>
       </c>
-      <c r="C40" s="38">
+      <c r="C40" s="35">
         <v>500000</v>
       </c>
       <c r="D40" s="22">
         <f t="shared" si="0"/>
         <v>139.85899800000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
+      <c r="E40" s="30">
+        <v>28</v>
+      </c>
+      <c r="F40" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="38">
+      <c r="B41" s="35">
         <v>69939538</v>
       </c>
-      <c r="C41" s="38">
+      <c r="C41" s="35">
         <v>500000</v>
       </c>
       <c r="D41" s="22">
         <f t="shared" si="0"/>
         <v>139.879076</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
+      <c r="E41" s="30">
+        <v>28</v>
+      </c>
+      <c r="F41" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="38">
+      <c r="B42" s="35">
         <v>69934497</v>
       </c>
-      <c r="C42" s="38">
+      <c r="C42" s="35">
         <v>500000</v>
       </c>
       <c r="D42" s="22">
         <f t="shared" si="0"/>
         <v>139.86899399999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+      <c r="E42" s="30">
+        <v>28</v>
+      </c>
+      <c r="F42" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="38">
+      <c r="B43" s="35">
         <v>69936203</v>
       </c>
-      <c r="C43" s="38">
+      <c r="C43" s="35">
         <v>500000</v>
       </c>
       <c r="D43" s="22">
         <f t="shared" si="0"/>
         <v>139.87240600000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
+      <c r="E43" s="30">
+        <v>28</v>
+      </c>
+      <c r="F43" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="38">
+      <c r="B44" s="35">
         <v>69970313</v>
       </c>
-      <c r="C44" s="38">
+      <c r="C44" s="35">
         <v>500000</v>
       </c>
       <c r="D44" s="22">
         <f t="shared" si="0"/>
         <v>139.94062600000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
+      <c r="E44" s="30">
+        <v>28</v>
+      </c>
+      <c r="F44" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="38">
+      <c r="B45" s="35">
         <v>69940096</v>
       </c>
-      <c r="C45" s="38">
+      <c r="C45" s="35">
         <v>500000</v>
       </c>
       <c r="D45" s="22">
         <f t="shared" si="0"/>
         <v>139.88019199999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+      <c r="E45" s="30">
+        <v>28</v>
+      </c>
+      <c r="F45" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="38">
+      <c r="B46" s="35">
         <v>69931107</v>
       </c>
-      <c r="C46" s="38">
+      <c r="C46" s="35">
         <v>500000</v>
       </c>
       <c r="D46" s="22">
         <f t="shared" si="0"/>
         <v>139.86221399999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="E46" s="30">
+        <v>28</v>
+      </c>
+      <c r="F46" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="38">
+      <c r="B47" s="35">
         <v>69937712</v>
       </c>
-      <c r="C47" s="38">
+      <c r="C47" s="35">
         <v>500000</v>
       </c>
       <c r="D47" s="22">
         <f t="shared" si="0"/>
         <v>139.87542400000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
+      <c r="E47" s="30">
+        <v>28</v>
+      </c>
+      <c r="F47" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="38">
+      <c r="B48" s="35">
         <v>69972723</v>
       </c>
-      <c r="C48" s="38">
+      <c r="C48" s="35">
         <v>500000</v>
       </c>
       <c r="D48" s="22">
         <f t="shared" si="0"/>
         <v>139.945446</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
+      <c r="E48" s="30">
+        <v>28</v>
+      </c>
+      <c r="F48" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B49" s="38">
+      <c r="B49" s="35">
         <v>77575286</v>
       </c>
-      <c r="C49" s="38">
+      <c r="C49" s="35">
         <v>500000</v>
       </c>
       <c r="D49" s="22">
         <f t="shared" si="0"/>
         <v>155.15057200000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+      <c r="E49" s="30">
+        <v>28</v>
+      </c>
+      <c r="F49" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="38">
+      <c r="B50" s="35">
         <v>84198846</v>
       </c>
-      <c r="C50" s="38">
+      <c r="C50" s="35">
         <v>500000</v>
       </c>
       <c r="D50" s="22">
         <f t="shared" si="0"/>
         <v>168.39769200000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
+      <c r="E50" s="30">
+        <v>28</v>
+      </c>
+      <c r="F50" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="38">
+      <c r="B51" s="35">
         <v>69905384</v>
       </c>
-      <c r="C51" s="38">
+      <c r="C51" s="35">
         <v>500000</v>
       </c>
       <c r="D51" s="22">
         <f t="shared" si="0"/>
         <v>139.810768</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+      <c r="E51" s="30">
+        <v>28</v>
+      </c>
+      <c r="F51" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="38">
+      <c r="B52" s="35">
         <v>69909786</v>
       </c>
-      <c r="C52" s="38">
+      <c r="C52" s="35">
         <v>500000</v>
       </c>
       <c r="D52" s="22">
         <f t="shared" si="0"/>
         <v>139.81957199999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+      <c r="E52" s="30">
+        <v>28</v>
+      </c>
+      <c r="F52" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="38">
+      <c r="B53" s="35">
         <v>69919169</v>
       </c>
-      <c r="C53" s="38">
+      <c r="C53" s="35">
         <v>500000</v>
       </c>
       <c r="D53" s="22">
         <f t="shared" si="0"/>
         <v>139.83833799999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+      <c r="E53" s="30">
+        <v>28</v>
+      </c>
+      <c r="F53" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="38">
+      <c r="B54" s="35">
         <v>69901238</v>
       </c>
-      <c r="C54" s="38">
+      <c r="C54" s="35">
         <v>500000</v>
       </c>
       <c r="D54" s="22">
         <f t="shared" si="0"/>
         <v>139.80247600000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
+      <c r="E54" s="30">
+        <v>28</v>
+      </c>
+      <c r="F54" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B55" s="38">
+      <c r="B55" s="35">
         <v>93464633</v>
       </c>
-      <c r="C55" s="38">
+      <c r="C55" s="35">
         <v>500000</v>
       </c>
       <c r="D55" s="22">
         <f t="shared" si="0"/>
         <v>186.92926600000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
+      <c r="E55" s="30">
+        <v>28</v>
+      </c>
+      <c r="F55" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="38">
+      <c r="B56" s="35">
         <v>104525166</v>
       </c>
-      <c r="C56" s="38">
+      <c r="C56" s="35">
         <v>500000</v>
       </c>
       <c r="D56" s="22">
         <f t="shared" si="0"/>
         <v>209.050332</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+      <c r="E56" s="30">
+        <v>28</v>
+      </c>
+      <c r="F56" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B57" s="38">
+      <c r="B57" s="35">
         <v>69951861</v>
       </c>
-      <c r="C57" s="38">
+      <c r="C57" s="35">
         <v>500000</v>
       </c>
       <c r="D57" s="22">
         <f t="shared" si="0"/>
         <v>139.90372199999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="33" t="s">
+      <c r="E57" s="30">
+        <v>28</v>
+      </c>
+      <c r="F57" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="38">
+      <c r="B58" s="35">
         <v>69915198</v>
       </c>
-      <c r="C58" s="38">
+      <c r="C58" s="35">
         <v>500000</v>
       </c>
       <c r="D58" s="22">
         <f t="shared" si="0"/>
         <v>139.83039600000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
+      <c r="E58" s="30">
+        <v>28</v>
+      </c>
+      <c r="F58" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B59" s="38">
+      <c r="B59" s="35">
         <v>69916773</v>
       </c>
-      <c r="C59" s="38">
+      <c r="C59" s="35">
         <v>500000</v>
       </c>
       <c r="D59" s="22">
         <f t="shared" si="0"/>
         <v>139.83354600000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="33" t="s">
+      <c r="E59" s="30">
+        <v>28</v>
+      </c>
+      <c r="F59" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="38">
+      <c r="B60" s="35">
         <v>69922018</v>
       </c>
-      <c r="C60" s="38">
+      <c r="C60" s="35">
         <v>500000</v>
       </c>
       <c r="D60" s="22">
         <f t="shared" si="0"/>
         <v>139.84403599999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+      <c r="E60" s="30">
+        <v>28</v>
+      </c>
+      <c r="F60" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B61" s="38">
+      <c r="B61" s="35">
         <v>94901338</v>
       </c>
-      <c r="C61" s="38">
+      <c r="C61" s="35">
         <v>500000</v>
       </c>
       <c r="D61" s="22">
         <f t="shared" si="0"/>
         <v>189.80267599999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="33" t="s">
+      <c r="E61" s="30">
+        <v>28</v>
+      </c>
+      <c r="F61" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="38">
+      <c r="B62" s="35">
         <v>114297440</v>
       </c>
-      <c r="C62" s="38">
+      <c r="C62" s="35">
         <v>500000</v>
       </c>
       <c r="D62" s="22">
         <f t="shared" si="0"/>
         <v>228.59487999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="33" t="s">
+      <c r="E62" s="30">
+        <v>28</v>
+      </c>
+      <c r="F62" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="38">
+      <c r="B63" s="35">
         <v>107262171</v>
       </c>
-      <c r="C63" s="38">
+      <c r="C63" s="35">
         <v>500000</v>
       </c>
       <c r="D63" s="22">
         <f t="shared" si="0"/>
         <v>214.52434199999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="33" t="s">
+      <c r="E63" s="30">
+        <v>28</v>
+      </c>
+      <c r="F63" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="38">
+      <c r="B64" s="35">
         <v>114737314</v>
       </c>
-      <c r="C64" s="38">
+      <c r="C64" s="35">
         <v>500000</v>
       </c>
       <c r="D64" s="22">
         <f t="shared" si="0"/>
         <v>229.474628</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="33" t="s">
+      <c r="E64" s="30">
+        <v>28</v>
+      </c>
+      <c r="F64" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="38">
+      <c r="B65" s="35">
         <v>99686925</v>
       </c>
-      <c r="C65" s="38">
+      <c r="C65" s="35">
         <v>500000</v>
       </c>
       <c r="D65" s="22">
         <f t="shared" si="0"/>
         <v>199.37385</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="33" t="s">
+      <c r="E65" s="30">
+        <v>28</v>
+      </c>
+      <c r="F65" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B66" s="38">
+      <c r="B66" s="35">
         <v>105947634</v>
       </c>
-      <c r="C66" s="38">
+      <c r="C66" s="35">
         <v>500000</v>
       </c>
       <c r="D66" s="22">
         <f t="shared" si="0"/>
         <v>211.89526799999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="33" t="s">
+      <c r="E66" s="30">
+        <v>28</v>
+      </c>
+      <c r="F66" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B67" s="38">
+      <c r="B67" s="35">
         <v>112424850</v>
       </c>
-      <c r="C67" s="38">
+      <c r="C67" s="35">
         <v>500000</v>
       </c>
       <c r="D67" s="22">
         <f t="shared" si="0"/>
         <v>224.84970000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
+      <c r="E67" s="30">
+        <v>28</v>
+      </c>
+      <c r="F67" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="B68" s="38">
+      <c r="B68" s="35">
         <v>103454867</v>
       </c>
-      <c r="C68" s="38">
+      <c r="C68" s="35">
         <v>500000</v>
       </c>
       <c r="D68" s="22">
         <f t="shared" si="0"/>
         <v>206.90973399999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="33" t="s">
+      <c r="E68" s="30">
+        <v>28</v>
+      </c>
+      <c r="F68" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="B69" s="38">
+      <c r="B69" s="35">
         <v>105195383</v>
       </c>
-      <c r="C69" s="38">
+      <c r="C69" s="35">
         <v>500000</v>
       </c>
       <c r="D69" s="22">
         <f t="shared" si="0"/>
         <v>210.39076600000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="33" t="s">
+      <c r="E69" s="30">
+        <v>28</v>
+      </c>
+      <c r="F69" s="30">
+        <f t="shared" si="1"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B70" s="38">
+      <c r="B70" s="35">
         <v>103821763</v>
       </c>
-      <c r="C70" s="38">
+      <c r="C70" s="35">
         <v>500000</v>
       </c>
       <c r="D70" s="22">
-        <f t="shared" ref="D70:D106" si="1">B70/C70</f>
+        <f t="shared" ref="D70:D106" si="2">B70/C70</f>
         <v>207.64352600000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="33" t="s">
+      <c r="E70" s="30">
+        <v>28</v>
+      </c>
+      <c r="F70" s="30">
+        <f t="shared" ref="F70:F106" si="3">C70/E70</f>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="B71" s="38">
+      <c r="B71" s="35">
         <v>91035050</v>
       </c>
-      <c r="C71" s="38">
+      <c r="C71" s="35">
         <v>500000</v>
       </c>
       <c r="D71" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>182.0701</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="33" t="s">
+      <c r="E71" s="30">
+        <v>28</v>
+      </c>
+      <c r="F71" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B72" s="38">
+      <c r="B72" s="35">
         <v>99498163</v>
       </c>
-      <c r="C72" s="38">
+      <c r="C72" s="35">
         <v>500000</v>
       </c>
       <c r="D72" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198.99632600000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="33" t="s">
+      <c r="E72" s="30">
+        <v>28</v>
+      </c>
+      <c r="F72" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="38">
+      <c r="B73" s="35">
         <v>102292773</v>
       </c>
-      <c r="C73" s="38">
+      <c r="C73" s="35">
         <v>500000</v>
       </c>
       <c r="D73" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>204.58554599999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="33" t="s">
+      <c r="E73" s="30">
+        <v>28</v>
+      </c>
+      <c r="F73" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B74" s="38">
+      <c r="B74" s="35">
         <v>98777448</v>
       </c>
-      <c r="C74" s="38">
+      <c r="C74" s="35">
         <v>500000</v>
       </c>
       <c r="D74" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>197.55489600000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="33" t="s">
+      <c r="E74" s="30">
+        <v>28</v>
+      </c>
+      <c r="F74" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="B75" s="38">
+      <c r="B75" s="35">
         <v>92426745</v>
       </c>
-      <c r="C75" s="38">
+      <c r="C75" s="35">
         <v>500000</v>
       </c>
       <c r="D75" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>184.85348999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+      <c r="E75" s="30">
+        <v>28</v>
+      </c>
+      <c r="F75" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="38">
+      <c r="B76" s="35">
         <v>105949676</v>
       </c>
-      <c r="C76" s="38">
+      <c r="C76" s="35">
         <v>500000</v>
       </c>
       <c r="D76" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>211.89935199999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="33" t="s">
+      <c r="E76" s="30">
+        <v>28</v>
+      </c>
+      <c r="F76" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B77" s="38">
+      <c r="B77" s="35">
         <v>99195546</v>
       </c>
-      <c r="C77" s="38">
+      <c r="C77" s="35">
         <v>500000</v>
       </c>
       <c r="D77" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198.39109199999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="33" t="s">
+      <c r="E77" s="30">
+        <v>28</v>
+      </c>
+      <c r="F77" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B78" s="38">
+      <c r="B78" s="35">
         <v>100381998</v>
       </c>
-      <c r="C78" s="38">
+      <c r="C78" s="35">
         <v>500000</v>
       </c>
       <c r="D78" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200.76399599999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="33" t="s">
+      <c r="E78" s="30">
+        <v>28</v>
+      </c>
+      <c r="F78" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B79" s="38">
+      <c r="B79" s="35">
         <v>101379736</v>
       </c>
-      <c r="C79" s="38">
+      <c r="C79" s="35">
         <v>500000</v>
       </c>
       <c r="D79" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>202.75947199999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="33" t="s">
+      <c r="E79" s="30">
+        <v>28</v>
+      </c>
+      <c r="F79" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="38">
+      <c r="B80" s="35">
         <v>97241294</v>
       </c>
-      <c r="C80" s="38">
+      <c r="C80" s="35">
         <v>500000</v>
       </c>
       <c r="D80" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>194.48258799999999</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="33" t="s">
+      <c r="E80" s="30">
+        <v>28</v>
+      </c>
+      <c r="F80" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="B81" s="38">
+      <c r="B81" s="35">
         <v>90319402</v>
       </c>
-      <c r="C81" s="38">
+      <c r="C81" s="35">
         <v>500000</v>
       </c>
       <c r="D81" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180.63880399999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+      <c r="E81" s="30">
+        <v>28</v>
+      </c>
+      <c r="F81" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B82" s="38">
+      <c r="B82" s="35">
         <v>90642493</v>
       </c>
-      <c r="C82" s="38">
+      <c r="C82" s="35">
         <v>500000</v>
       </c>
       <c r="D82" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>181.284986</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="33" t="s">
+      <c r="E82" s="30">
+        <v>28</v>
+      </c>
+      <c r="F82" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="B83" s="38">
+      <c r="B83" s="35">
         <v>97537714</v>
       </c>
-      <c r="C83" s="38">
+      <c r="C83" s="35">
         <v>500000</v>
       </c>
       <c r="D83" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>195.07542799999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="33" t="s">
+      <c r="E83" s="30">
+        <v>28</v>
+      </c>
+      <c r="F83" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="B84" s="38">
+      <c r="B84" s="35">
         <v>98884601</v>
       </c>
-      <c r="C84" s="38">
+      <c r="C84" s="35">
         <v>500000</v>
       </c>
       <c r="D84" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>197.76920200000001</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="33" t="s">
+      <c r="E84" s="30">
+        <v>28</v>
+      </c>
+      <c r="F84" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B85" s="38">
+      <c r="B85" s="35">
         <v>91902456</v>
       </c>
-      <c r="C85" s="38">
+      <c r="C85" s="35">
         <v>500000</v>
       </c>
       <c r="D85" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>183.804912</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="33" t="s">
+      <c r="E85" s="30">
+        <v>28</v>
+      </c>
+      <c r="F85" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="B86" s="38">
+      <c r="B86" s="35">
         <v>99851880</v>
       </c>
-      <c r="C86" s="38">
+      <c r="C86" s="35">
         <v>500000</v>
       </c>
       <c r="D86" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>199.70375999999999</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="33" t="s">
+      <c r="E86" s="30">
+        <v>28</v>
+      </c>
+      <c r="F86" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B87" s="38">
+      <c r="B87" s="35">
         <v>97182369</v>
       </c>
-      <c r="C87" s="38">
+      <c r="C87" s="35">
         <v>500000</v>
       </c>
       <c r="D87" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>194.36473799999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="33" t="s">
+      <c r="E87" s="30">
+        <v>28</v>
+      </c>
+      <c r="F87" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="B88" s="38">
+      <c r="B88" s="35">
         <v>111682088</v>
       </c>
-      <c r="C88" s="38">
+      <c r="C88" s="35">
         <v>500000</v>
       </c>
       <c r="D88" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>223.36417599999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="33" t="s">
+      <c r="E88" s="30">
+        <v>28</v>
+      </c>
+      <c r="F88" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="B89" s="38">
+      <c r="B89" s="35">
         <v>97228019</v>
       </c>
-      <c r="C89" s="38">
+      <c r="C89" s="35">
         <v>500000</v>
       </c>
       <c r="D89" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>194.45603800000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="33" t="s">
+      <c r="E89" s="30">
+        <v>28</v>
+      </c>
+      <c r="F89" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="38">
+      <c r="B90" s="35">
         <v>116928690</v>
       </c>
-      <c r="C90" s="38">
+      <c r="C90" s="35">
         <v>500000</v>
       </c>
       <c r="D90" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>233.85738000000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="33" t="s">
+      <c r="E90" s="30">
+        <v>28</v>
+      </c>
+      <c r="F90" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B91" s="38">
+      <c r="B91" s="35">
         <v>238350844</v>
       </c>
-      <c r="C91" s="38">
+      <c r="C91" s="35">
         <v>500000</v>
       </c>
       <c r="D91" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>476.70168799999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="33" t="s">
+      <c r="E91" s="30">
+        <v>28</v>
+      </c>
+      <c r="F91" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B92" s="38">
+      <c r="B92" s="35">
         <v>119463297</v>
       </c>
-      <c r="C92" s="38">
+      <c r="C92" s="35">
         <v>500000</v>
       </c>
       <c r="D92" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>238.92659399999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="33" t="s">
+      <c r="E92" s="30">
+        <v>28</v>
+      </c>
+      <c r="F92" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="B93" s="38">
+      <c r="B93" s="35">
         <v>189803147</v>
       </c>
-      <c r="C93" s="38">
+      <c r="C93" s="35">
         <v>500000</v>
       </c>
       <c r="D93" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>379.60629399999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="33" t="s">
+      <c r="E93" s="30">
+        <v>28</v>
+      </c>
+      <c r="F93" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="B94" s="38">
+      <c r="B94" s="35">
         <v>233229533</v>
       </c>
-      <c r="C94" s="38">
+      <c r="C94" s="35">
         <v>500000</v>
       </c>
       <c r="D94" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>466.45906600000001</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="33" t="s">
+      <c r="E94" s="30">
+        <v>28</v>
+      </c>
+      <c r="F94" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B95" s="38">
+      <c r="B95" s="35">
         <v>218441522</v>
       </c>
-      <c r="C95" s="38">
+      <c r="C95" s="35">
         <v>500000</v>
       </c>
       <c r="D95" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>436.88304399999998</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="33" t="s">
+      <c r="E95" s="30">
+        <v>28</v>
+      </c>
+      <c r="F95" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="B96" s="38">
+      <c r="B96" s="35">
         <v>216072658</v>
       </c>
-      <c r="C96" s="38">
+      <c r="C96" s="35">
         <v>500000</v>
       </c>
       <c r="D96" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>432.14531599999998</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="33" t="s">
+      <c r="E96" s="30">
+        <v>28</v>
+      </c>
+      <c r="F96" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B97" s="38">
+      <c r="B97" s="35">
         <v>134970172</v>
       </c>
-      <c r="C97" s="38">
+      <c r="C97" s="35">
         <v>500000</v>
       </c>
       <c r="D97" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>269.94034399999998</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="33" t="s">
+      <c r="E97" s="30">
+        <v>28</v>
+      </c>
+      <c r="F97" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="38">
+      <c r="B98" s="35">
         <v>107431604</v>
       </c>
-      <c r="C98" s="38">
+      <c r="C98" s="35">
         <v>500000</v>
       </c>
       <c r="D98" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>214.86320799999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="33" t="s">
+      <c r="E98" s="30">
+        <v>28</v>
+      </c>
+      <c r="F98" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B99" s="38">
+      <c r="B99" s="35">
         <v>113652706</v>
       </c>
-      <c r="C99" s="38">
+      <c r="C99" s="35">
         <v>500000</v>
       </c>
       <c r="D99" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>227.30541199999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+      <c r="E99" s="30">
+        <v>28</v>
+      </c>
+      <c r="F99" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="B100" s="38">
+      <c r="B100" s="35">
         <v>158672195</v>
       </c>
-      <c r="C100" s="38">
+      <c r="C100" s="35">
         <v>500000</v>
       </c>
       <c r="D100" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>317.34438999999998</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="33" t="s">
+      <c r="E100" s="30">
+        <v>28</v>
+      </c>
+      <c r="F100" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B101" s="38">
+      <c r="B101" s="35">
         <v>283750086</v>
       </c>
-      <c r="C101" s="38">
+      <c r="C101" s="35">
         <v>500000</v>
       </c>
       <c r="D101" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>567.50017200000002</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="33" t="s">
+      <c r="E101" s="30">
+        <v>28</v>
+      </c>
+      <c r="F101" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B102" s="38">
+      <c r="B102" s="35">
         <v>206954008</v>
       </c>
-      <c r="C102" s="38">
+      <c r="C102" s="35">
         <v>500000</v>
       </c>
       <c r="D102" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>413.90801599999998</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="33" t="s">
+      <c r="E102" s="30">
+        <v>28</v>
+      </c>
+      <c r="F102" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="B103" s="38">
+      <c r="B103" s="35">
         <v>206952024</v>
       </c>
-      <c r="C103" s="38">
+      <c r="C103" s="35">
         <v>500000</v>
       </c>
       <c r="D103" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>413.90404799999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="33" t="s">
+      <c r="E103" s="30">
+        <v>28</v>
+      </c>
+      <c r="F103" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B104" s="38">
+      <c r="B104" s="35">
         <v>206960360</v>
       </c>
-      <c r="C104" s="38">
+      <c r="C104" s="35">
         <v>500000</v>
       </c>
       <c r="D104" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>413.92072000000002</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="33" t="s">
+      <c r="E104" s="30">
+        <v>28</v>
+      </c>
+      <c r="F104" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="B105" s="38">
+      <c r="B105" s="35">
         <v>206968130</v>
       </c>
-      <c r="C105" s="38">
+      <c r="C105" s="35">
         <v>500000</v>
       </c>
       <c r="D105" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>413.93626</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="34" t="s">
+      <c r="E105" s="30">
+        <v>28</v>
+      </c>
+      <c r="F105" s="30">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="B106" s="39">
+      <c r="B106" s="36">
         <v>145543574</v>
       </c>
-      <c r="C106" s="39">
-        <v>500000</v>
-      </c>
-      <c r="D106" s="36">
-        <f t="shared" si="1"/>
+      <c r="C106" s="36">
+        <v>500000</v>
+      </c>
+      <c r="D106" s="33">
+        <f t="shared" si="2"/>
         <v>291.08714800000001</v>
+      </c>
+      <c r="E106" s="31">
+        <v>28</v>
+      </c>
+      <c r="F106" s="31">
+        <f t="shared" si="3"/>
+        <v>17857.142857142859</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>